<commit_message>
add gis messy dataset
</commit_message>
<xml_diff>
--- a/intro_course/data/raw/messy_data_examples.xlsx
+++ b/intro_course/data/raw/messy_data_examples.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neale\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neale\Documents\Applied Epi\repos\intro_course\intro_course\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F9DCE3C-3B75-4150-9882-45774E1124B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16803891-AA73-4317-914E-1391B90FE4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1640" yWindow="1520" windowWidth="17120" windowHeight="7270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="messy_colors" sheetId="1" r:id="rId1"/>
-    <sheet name="messy_site_coverage_1" sheetId="3" r:id="rId2"/>
-    <sheet name="messy_site_coverage_2" sheetId="4" r:id="rId3"/>
-    <sheet name="tidy_site_coverage" sheetId="2" r:id="rId4"/>
+    <sheet name="messy_site_coverage" sheetId="3" r:id="rId2"/>
+    <sheet name="tidy_site_coverage" sheetId="2" r:id="rId3"/>
+    <sheet name="messy_gis" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="108">
   <si>
     <t>Province</t>
   </si>
@@ -314,6 +314,105 @@
   <si>
     <t>Site coverage - May and June 2022</t>
   </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Treatment Center</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Location General</t>
+  </si>
+  <si>
+    <t>GPS</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>Number of Beds</t>
+  </si>
+  <si>
+    <t>Patients</t>
+  </si>
+  <si>
+    <t>Operative</t>
+  </si>
+  <si>
+    <t>CTC</t>
+  </si>
+  <si>
+    <t>Site A</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>S25°10'08.0"</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>E012°19'03.7"</t>
+  </si>
+  <si>
+    <t>Site B</t>
+  </si>
+  <si>
+    <t>S25°10'37.4"</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>E012°19'25.4"</t>
+  </si>
+  <si>
+    <t>CTU</t>
+  </si>
+  <si>
+    <t>Site C</t>
+  </si>
+  <si>
+    <t>S25°10'25.8"</t>
+  </si>
+  <si>
+    <t>E012°19'35.1"</t>
+  </si>
+  <si>
+    <t>Site D</t>
+  </si>
+  <si>
+    <t>S25°10'76.3"</t>
+  </si>
+  <si>
+    <t>E010°19'83.6"</t>
+  </si>
+  <si>
+    <t>Site E</t>
+  </si>
+  <si>
+    <t>Rural</t>
+  </si>
+  <si>
+    <t>25°10'81.7"</t>
+  </si>
+  <si>
+    <t>E010°19'63.7"</t>
+  </si>
+  <si>
+    <t>Planned (F)</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Site G</t>
+  </si>
 </sst>
 </file>
 
@@ -322,7 +421,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,8 +528,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,6 +597,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -545,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -642,7 +754,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -662,6 +773,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -947,7 +1071,7 @@
   <dimension ref="B3:Y32"/>
   <sheetViews>
     <sheetView topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
@@ -995,30 +1119,30 @@
       <c r="E4" s="4"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="41"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
       <c r="T4" s="8"/>
       <c r="U4" s="14"/>
     </row>
     <row r="5" spans="2:25" s="9" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="4"/>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8" t="s">
@@ -2006,7 +2130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FAE9F5F-3B9F-45D4-AF0F-FEC4E68A1532}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
@@ -2018,31 +2142,31 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="39" t="s">
         <v>7</v>
       </c>
@@ -2143,7 +2267,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="42" t="s">
         <v>68</v>
       </c>
       <c r="B5" s="37">
@@ -2168,7 +2292,7 @@
       <c r="Q5" s="37"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" s="43"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="37">
         <v>2</v>
       </c>
@@ -2189,16 +2313,16 @@
       <c r="Q6" s="37"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" s="43"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="37">
         <v>3</v>
       </c>
       <c r="C7" s="37"/>
       <c r="D7" s="37"/>
-      <c r="E7" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="44"/>
+      <c r="E7" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="43"/>
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -2212,7 +2336,7 @@
       <c r="Q7" s="37"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" s="43"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="37">
         <v>4</v>
       </c>
@@ -2235,7 +2359,7 @@
       <c r="Q8" s="37"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" s="43"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="37">
         <v>5</v>
       </c>
@@ -2243,24 +2367,24 @@
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
-      <c r="G9" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
+      <c r="G9" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
       <c r="L9" s="37"/>
-      <c r="M9" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="N9" s="44"/>
-      <c r="O9" s="44"/>
+      <c r="M9" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
       <c r="P9" s="37"/>
       <c r="Q9" s="37"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A10" s="43"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="37">
         <v>6</v>
       </c>
@@ -2281,7 +2405,7 @@
       <c r="Q10" s="37"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A11" s="43"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="37">
         <v>7</v>
       </c>
@@ -2310,7 +2434,7 @@
       <c r="Q11" s="37"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="42" t="s">
         <v>69</v>
       </c>
       <c r="B12" s="37">
@@ -2335,7 +2459,7 @@
       <c r="Q12" s="37"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="43"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="37">
         <v>9</v>
       </c>
@@ -2356,22 +2480,22 @@
       <c r="Q13" s="37"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A14" s="43"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="37">
         <v>10</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="37"/>
-      <c r="E14" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="44"/>
+      <c r="E14" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="43"/>
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
-      <c r="I14" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="J14" s="44"/>
+      <c r="I14" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="J14" s="43"/>
       <c r="K14" s="37"/>
       <c r="L14" s="37"/>
       <c r="M14" s="37"/>
@@ -2381,7 +2505,7 @@
       <c r="Q14" s="37"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="43"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="37">
         <v>11</v>
       </c>
@@ -2406,7 +2530,7 @@
       <c r="Q15" s="37"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A16" s="43"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="37">
         <v>12</v>
       </c>
@@ -2414,24 +2538,24 @@
       <c r="D16" s="37"/>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
-      <c r="G16" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
+      <c r="G16" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
       <c r="L16" s="37"/>
-      <c r="M16" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="N16" s="44"/>
-      <c r="O16" s="44"/>
+      <c r="M16" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="N16" s="43"/>
+      <c r="O16" s="43"/>
       <c r="P16" s="37"/>
       <c r="Q16" s="37"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A17" s="43"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="37">
         <v>13</v>
       </c>
@@ -2452,7 +2576,7 @@
       <c r="Q17" s="37"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A18" s="43"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="37">
         <v>14</v>
       </c>
@@ -2500,509 +2624,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28477882-8086-4076-8817-80CD194A9235}">
-  <dimension ref="A1:Q18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:17" ht="31" x14ac:dyDescent="0.7">
-      <c r="A1" s="36" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="O3" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" s="39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="39">
-        <v>31</v>
-      </c>
-      <c r="D4" s="39">
-        <v>1</v>
-      </c>
-      <c r="E4" s="39">
-        <v>2</v>
-      </c>
-      <c r="F4" s="39">
-        <v>3</v>
-      </c>
-      <c r="G4" s="39">
-        <v>4</v>
-      </c>
-      <c r="H4" s="39">
-        <v>5</v>
-      </c>
-      <c r="I4" s="39">
-        <v>6</v>
-      </c>
-      <c r="J4" s="39">
-        <v>7</v>
-      </c>
-      <c r="K4" s="39">
-        <v>8</v>
-      </c>
-      <c r="L4" s="39">
-        <v>9</v>
-      </c>
-      <c r="M4" s="39">
-        <v>10</v>
-      </c>
-      <c r="N4" s="39">
-        <v>11</v>
-      </c>
-      <c r="O4" s="39">
-        <v>12</v>
-      </c>
-      <c r="P4" s="39">
-        <v>13</v>
-      </c>
-      <c r="Q4" s="39">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="37">
-        <v>1</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" s="43"/>
-      <c r="B6" s="37">
-        <v>2</v>
-      </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" s="43"/>
-      <c r="B7" s="37">
-        <v>3</v>
-      </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" s="43"/>
-      <c r="B8" s="37">
-        <v>4</v>
-      </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" s="43"/>
-      <c r="B9" s="37">
-        <v>5</v>
-      </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="I9" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="J9" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="K9" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="L9" s="37"/>
-      <c r="M9" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="N9" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="O9" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="37"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A10" s="43"/>
-      <c r="B10" s="37">
-        <v>6</v>
-      </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="37"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A11" s="43"/>
-      <c r="B11" s="37">
-        <v>7</v>
-      </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" s="37"/>
-      <c r="J11" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="37"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="37">
-        <v>8</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="37"/>
-      <c r="P12" s="37"/>
-      <c r="Q12" s="37"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="43"/>
-      <c r="B13" s="37">
-        <v>9</v>
-      </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="37"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A14" s="43"/>
-      <c r="B14" s="37">
-        <v>10</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="44"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="43"/>
-      <c r="B15" s="37">
-        <v>11</v>
-      </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A16" s="43"/>
-      <c r="B16" s="37">
-        <v>12</v>
-      </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="N16" s="44"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="37"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A17" s="43"/>
-      <c r="B17" s="37">
-        <v>13</v>
-      </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A18" s="43"/>
-      <c r="B18" s="37">
-        <v>14</v>
-      </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="37"/>
-      <c r="F18" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="G18" s="37"/>
-      <c r="H18" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="I18" s="37"/>
-      <c r="J18" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
-    </row>
-  </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:A11"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5891AB96-3640-4460-AA71-501ACCEF12FC}">
   <dimension ref="A1:D36"/>
   <sheetViews>
@@ -3523,4 +3144,438 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F7E83F-CF9D-41EE-BEEB-68CA7E654CC0}">
+  <dimension ref="A2:Q17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:Q17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="48">
+        <v>1</v>
+      </c>
+      <c r="B4" s="47"/>
+      <c r="C4" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="47"/>
+      <c r="E4" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="47"/>
+      <c r="G4" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="47"/>
+      <c r="I4" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="J4" s="47"/>
+      <c r="K4" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="47"/>
+      <c r="M4" s="48">
+        <v>80</v>
+      </c>
+      <c r="N4" s="47"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="47"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="48">
+        <v>2</v>
+      </c>
+      <c r="B6" s="47"/>
+      <c r="C6" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="47"/>
+      <c r="E6" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="47"/>
+      <c r="G6" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" s="47"/>
+      <c r="I6" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" s="47"/>
+      <c r="K6" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="47"/>
+      <c r="M6" s="48">
+        <v>150</v>
+      </c>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="47"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="48">
+        <v>3</v>
+      </c>
+      <c r="B8" s="47"/>
+      <c r="C8" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="47"/>
+      <c r="G8" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" s="47"/>
+      <c r="I8" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="J8" s="47"/>
+      <c r="K8" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" s="47"/>
+      <c r="M8" s="48">
+        <v>19</v>
+      </c>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="47"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="48">
+        <v>4</v>
+      </c>
+      <c r="B10" s="47"/>
+      <c r="C10" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="47"/>
+      <c r="E10" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="47"/>
+      <c r="G10" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" s="47"/>
+      <c r="I10" s="48" t="s">
+        <v>99</v>
+      </c>
+      <c r="J10" s="47"/>
+      <c r="K10" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" s="47"/>
+      <c r="M10" s="48">
+        <v>50</v>
+      </c>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="47"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="48">
+        <v>5</v>
+      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="F12" s="47"/>
+      <c r="G12" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" s="47"/>
+      <c r="I12" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" s="47"/>
+      <c r="K12" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12" s="47"/>
+      <c r="M12" s="48">
+        <v>10</v>
+      </c>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="47"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="47"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="50">
+        <v>6</v>
+      </c>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50">
+        <v>150</v>
+      </c>
+      <c r="N14" s="50"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="50" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="47"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="48">
+        <v>7</v>
+      </c>
+      <c r="B16" s="47"/>
+      <c r="C16" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="47"/>
+      <c r="E16" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="47"/>
+      <c r="G16" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47">
+        <v>-25.61487</v>
+      </c>
+      <c r="J16" s="47"/>
+      <c r="K16" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" s="47"/>
+      <c r="M16" s="48">
+        <v>20</v>
+      </c>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="51" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I17" s="47">
+        <v>10.7400299999999</v>
+      </c>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="51"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>